<commit_message>
rajout de la signature de l'auteur
</commit_message>
<xml_diff>
--- a/Analyse du site.xlsx
+++ b/Analyse du site.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ouali\OneDrive\Bureau\Projet  Panthère\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC38EEB1-DFEF-4DE8-8093-B56FE1296589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB4F673-A4D1-4F90-8A78-4A74447D5DC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
   <si>
     <t>Catégorie</t>
   </si>
@@ -525,7 +525,7 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -596,6 +596,9 @@
       </c>
       <c r="E2" s="6" t="s">
         <v>19</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>